<commit_message>
Correção de caminho da pasta de imagem
</commit_message>
<xml_diff>
--- a/@_SALVAR PLANILHA AQUI/Arquivo de exportação.xlsx
+++ b/@_SALVAR PLANILHA AQUI/Arquivo de exportação.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\marketing\Weslley\Script\Script de automação\@_SALVAR PLANILHA AQUI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\Script de automação\@_SALVAR PLANILHA AQUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,29 +29,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -71,22 +55,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -366,116 +341,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Plan3"/>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="3"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="3"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="3"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="3"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="3"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="3"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="3"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="3"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="3"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="3"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="3"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="3"/>
-      <c r="F12" s="1"/>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F15" s="1"/>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>